<commit_message>
Added functionality to actually draw from the data from the advanced settings table. Added some space for a diagram. Understood the problem within my thermal and mechanical advanced model so will be moving on to fixing that now
</commit_message>
<xml_diff>
--- a/programData/advancedSettings.xlsx
+++ b/programData/advancedSettings.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="110" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="138" uniqueCount="31">
   <si>
     <t>Component</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>909999</t>
+  </si>
+  <si>
+    <t>abc</t>
   </si>
 </sst>
 </file>
@@ -588,7 +591,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Added a button for reverting to default for advanced settings
</commit_message>
<xml_diff>
--- a/programData/advancedSettings.xlsx
+++ b/programData/advancedSettings.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="138" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="168" uniqueCount="33">
   <si>
     <t>Component</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>abc</t>
+  </si>
+  <si>
+    <t>Coefficient of thermal expansion (microstrain/K)</t>
+  </si>
+  <si>
+    <t>-1</t>
   </si>
 </sst>
 </file>
@@ -574,14 +580,18 @@
       <c r="A4" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.25">
       <c r="A5" s="0" t="s">
@@ -591,7 +601,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>22</v>
@@ -602,7 +612,7 @@
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.25">
       <c r="A6" s="0" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Cleared up the situation with where the variables in HSM come from. Added support for retrieving information from the advanced model's spectra
</commit_message>
<xml_diff>
--- a/programData/advancedSettings.xlsx
+++ b/programData/advancedSettings.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EG5565\programData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{345D2759-9886-4A7A-80B6-7FB4DB7071ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13314051-2C00-46B8-B314-4F48F9FC4648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3210" yWindow="1650" windowWidth="23505" windowHeight="13635"/>
+    <workbookView xWindow="29535" yWindow="1200" windowWidth="23505" windowHeight="13635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" fullCalcOnLoad="true"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,23 +36,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="198" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>Component</t>
   </si>
   <si>
-    <t>Optical Fiber</t>
-  </si>
-  <si>
     <t>Coating</t>
   </si>
   <si>
     <t>Adhesive</t>
   </si>
   <si>
-    <t>Host structure</t>
-  </si>
-  <si>
     <t>Young's Modulus (Gpa)</t>
   </si>
   <si>
@@ -125,23 +119,47 @@
     <t>HostStructure</t>
   </si>
   <si>
-    <t>909999</t>
-  </si>
-  <si>
-    <t>abc</t>
-  </si>
-  <si>
-    <t>Coefficient of thermal expansion (microstrain/K)</t>
-  </si>
-  <si>
     <t>-1</t>
+  </si>
+  <si>
+    <t>Refractive index</t>
+  </si>
+  <si>
+    <t>1.47</t>
+  </si>
+  <si>
+    <t>Thermo-optic coeff (ue/K)</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Grating period (um)</t>
+  </si>
+  <si>
+    <t>0.527212</t>
+  </si>
+  <si>
+    <t>HSMVals</t>
+  </si>
+  <si>
+    <t>HSMVars</t>
+  </si>
+  <si>
+    <t>Ref. temperature (deg C)</t>
+  </si>
+  <si>
+    <t>Fiber length (m)</t>
+  </si>
+  <si>
+    <t>0.0015</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,7 +177,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -167,15 +185,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -194,7 +210,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -345,7 +361,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -369,9 +385,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -395,7 +411,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -430,7 +446,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="false">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -448,7 +464,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -473,7 +489,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -509,122 +525,158 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1BC06A6-79CD-4371-A2F4-2F5240BC5FAC}">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1BC06A6-79CD-4371-A2F4-2F5240BC5FAC}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11" style="1" customWidth="true"/>
-    <col min="1" max="1" width="29" customWidth="true"/>
-    <col min="3" max="3" width="7.375" style="1" customWidth="true"/>
-    <col min="4" max="4" width="8.5" style="1" customWidth="true"/>
-    <col min="5" max="5" width="12.375" style="1" customWidth="true"/>
+    <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="2" max="2" width="11" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.25">
-      <c r="A2" s="0" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>26</v>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.25">
-      <c r="A3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>11</v>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.25">
-      <c r="A4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.25">
-      <c r="A5" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="1" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.25">
-      <c r="A6" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>20</v>
+      <c r="F6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -633,6 +685,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100226B45C32477CF489353B2CDA66FAC1B" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="417eff293c01dedf1bc0d3a0c76dbd30">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="535a45db-52dd-462d-b530-861a768bf350" xmlns:ns4="ed479123-7fc5-4802-b1d0-8595281d3bc0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cc1d592e64bf5b07b7ab1b0c38ecc7b1" ns3:_="" ns4:_="">
     <xsd:import namespace="535a45db-52dd-462d-b530-861a768bf350"/>
@@ -873,15 +934,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -891,6 +943,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40694726-4DC8-47C7-96EA-9D05C9BA6005}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F670EEB-087B-4BD5-9482-7F1B6ED22C36}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -909,14 +969,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40694726-4DC8-47C7-96EA-9D05C9BA6005}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2502B54-2402-40CA-8896-A60076B89A64}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Version 1.0 - features complete. Will continue polishing and attempting to find problems
</commit_message>
<xml_diff>
--- a/programData/advancedSettings.xlsx
+++ b/programData/advancedSettings.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,12 +10,12 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13314051-2C00-46B8-B314-4F48F9FC4648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29535" yWindow="1200" windowWidth="23505" windowHeight="13635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29535" yWindow="1200" windowWidth="23505" windowHeight="13635"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="84" uniqueCount="39">
   <si>
     <t>Component</t>
   </si>
@@ -158,8 +158,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,7 +177,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -185,13 +185,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -210,7 +212,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -361,7 +363,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -385,9 +387,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -411,7 +413,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -446,7 +448,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="false">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -464,7 +466,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -489,7 +491,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -525,24 +527,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1BC06A6-79CD-4371-A2F4-2F5240BC5FAC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1BC06A6-79CD-4371-A2F4-2F5240BC5FAC}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="11" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="29" customWidth="true"/>
+    <col min="2" max="2" width="11" style="1" customWidth="true"/>
+    <col min="3" max="3" width="7.375" style="1" customWidth="true"/>
+    <col min="4" max="4" width="8.5" style="1" customWidth="true"/>
+    <col min="5" max="5" width="12.375" style="1" customWidth="true"/>
+    <col min="6" max="6" width="8.625" customWidth="true"/>
+    <col min="7" max="7" width="22" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -564,8 +568,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.25">
+      <c r="A2" s="0" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -587,8 +591,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.25">
+      <c r="A3" s="0" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -610,8 +614,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.25">
+      <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -633,8 +637,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.25">
+      <c r="A5" s="0" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -656,8 +660,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.25">
+      <c r="A6" s="0" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="1" t="s">

</xml_diff>

<commit_message>
1.01. Fixed advanced method because I was a little silly and didn't notice it was broken until now
</commit_message>
<xml_diff>
--- a/programData/advancedSettings.xlsx
+++ b/programData/advancedSettings.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="84" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="126" uniqueCount="40">
   <si>
     <t>Component</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>0.0015</t>
+  </si>
+  <si>
+    <t>2.2</t>
   </si>
 </sst>
 </file>
@@ -622,7 +625,7 @@
         <v>27</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Fixed advanced method 2: minor logical error in simulate
</commit_message>
<xml_diff>
--- a/programData/advancedSettings.xlsx
+++ b/programData/advancedSettings.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="126" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="168" uniqueCount="41">
   <si>
     <t>Component</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>2.2</t>
+  </si>
+  <si>
+    <t>0.05</t>
   </si>
 </sst>
 </file>
@@ -654,7 +657,7 @@
         <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Changed defaults to be consistent with the suggested design
</commit_message>
<xml_diff>
--- a/programData/advancedSettings.xlsx
+++ b/programData/advancedSettings.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="168" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="420" uniqueCount="45">
   <si>
     <t>Component</t>
   </si>
@@ -159,6 +159,18 @@
   </si>
   <si>
     <t>0.05</t>
+  </si>
+  <si>
+    <t>199</t>
+  </si>
+  <si>
+    <t>0.55</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>8.6</t>
   </si>
 </sst>
 </file>
@@ -588,7 +600,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>29</v>
@@ -628,7 +640,7 @@
         <v>27</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>12</v>
@@ -637,7 +649,7 @@
         <v>27</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>30</v>
@@ -657,7 +669,7 @@
         <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>17</v>
@@ -671,7 +683,7 @@
         <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>16</v>
@@ -680,7 +692,7 @@
         <v>17</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>38</v>

</xml_diff>